<commit_message>
SE-1843: consolidated cost basis movements into single transaction
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasPartridge\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760A9E5A-4ED0-4725-A94A-4927EEAC379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B0DE4-1126-49D6-AB27-C17C0D1436C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="264" windowWidth="19344" windowHeight="13320" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
   <si>
     <t>trade_date</t>
   </si>
@@ -64,9 +64,6 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>contract_size</t>
-  </si>
-  <si>
     <t>tc</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>portfolio</t>
   </si>
   <si>
-    <t>FundsIn</t>
-  </si>
-  <si>
     <t>currency_id</t>
   </si>
   <si>
@@ -148,27 +142,15 @@
     <t>futa_txn_002</t>
   </si>
   <si>
-    <t>crdcb_txn_001</t>
-  </si>
-  <si>
-    <t>cshb_txn_001</t>
-  </si>
-  <si>
     <t>futb_txn_001</t>
   </si>
   <si>
     <t>futb_txn_002</t>
   </si>
   <si>
-    <t>StockOut</t>
-  </si>
-  <si>
     <t>2021-01-03T14:15:00Z</t>
   </si>
   <si>
-    <t>StockIn</t>
-  </si>
-  <si>
     <t>Day 3 intraday trade price</t>
   </si>
   <si>
@@ -181,19 +163,22 @@
     <t>FuturesPortfolioForPnLCalc</t>
   </si>
   <si>
-    <t>crdcb_txn_002</t>
-  </si>
-  <si>
-    <t>cshb_txn_002</t>
-  </si>
-  <si>
     <t>FUT_ICEOJZDEC21</t>
   </si>
   <si>
-    <t>-325000</t>
-  </si>
-  <si>
     <t>scaling_factor</t>
+  </si>
+  <si>
+    <t>RealisePnLIncrease</t>
+  </si>
+  <si>
+    <t>RealisePnLDecrease</t>
+  </si>
+  <si>
+    <t>rpnlb_txn_001</t>
+  </si>
+  <si>
+    <t>rpnbl_txn_002</t>
   </si>
 </sst>
 </file>
@@ -246,15 +231,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -576,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,11 +570,11 @@
     <col min="2" max="4" width="23.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5546875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="23.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -609,270 +591,197 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>10000000</v>
       </c>
-      <c r="I2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1">
         <v>99.5</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>4975000</v>
       </c>
-      <c r="I3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1">
         <v>100</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>10000000</v>
       </c>
-      <c r="I4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>50000</v>
       </c>
-      <c r="I5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="1">
-        <v>50000</v>
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5">
-        <v>50000</v>
-      </c>
-      <c r="J6" t="s">
+        <v>99.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4975000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1">
-        <v>99.5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>4975000</v>
-      </c>
-      <c r="I7" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>325000</v>
+      </c>
+      <c r="I7" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>325000</v>
-      </c>
-      <c r="I8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="5">
-        <v>325000</v>
-      </c>
-      <c r="J9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H11" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -909,430 +818,430 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1">
         <v>1E-4</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1">
         <v>1E-4</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F13" s="1">
         <v>1E-4</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14" s="1">
         <v>1E-4</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="1">
         <v>1E-4</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F16" s="1">
         <v>1E-4</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="1">
         <v>1E-4</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F18" s="1">
         <v>1E-4</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1">
         <v>1E-4</v>
       </c>
       <c r="G19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE-1843: Re-wrote notebook to use Bund Futures
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B0DE4-1126-49D6-AB27-C17C0D1436C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC7DDF2-1F91-4585-9EBE-7DAA401260E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Day 3 closing price</t>
   </si>
   <si>
-    <t>FUT_ICEKCZDEC21</t>
-  </si>
-  <si>
     <t>2021-01-01T17:00:00Z</t>
   </si>
   <si>
@@ -142,43 +139,46 @@
     <t>futa_txn_002</t>
   </si>
   <si>
+    <t>futb_txn_002</t>
+  </si>
+  <si>
+    <t>2021-01-03T14:15:00Z</t>
+  </si>
+  <si>
+    <t>Day 3 intraday trade price</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>ClientInternal</t>
+  </si>
+  <si>
+    <t>FuturesPortfolioForPnLCalc</t>
+  </si>
+  <si>
+    <t>scaling_factor</t>
+  </si>
+  <si>
+    <t>RealisePnLIncrease</t>
+  </si>
+  <si>
+    <t>RealisePnLDecrease</t>
+  </si>
+  <si>
+    <t>rpnlb_txn_001</t>
+  </si>
+  <si>
+    <t>rpnbl_txn_002</t>
+  </si>
+  <si>
+    <t>FutBob001</t>
+  </si>
+  <si>
+    <t>FutBob002</t>
+  </si>
+  <si>
     <t>futb_txn_001</t>
-  </si>
-  <si>
-    <t>futb_txn_002</t>
-  </si>
-  <si>
-    <t>2021-01-03T14:15:00Z</t>
-  </si>
-  <si>
-    <t>Day 3 intraday trade price</t>
-  </si>
-  <si>
-    <t>id_type</t>
-  </si>
-  <si>
-    <t>ClientInternal</t>
-  </si>
-  <si>
-    <t>FuturesPortfolioForPnLCalc</t>
-  </si>
-  <si>
-    <t>FUT_ICEOJZDEC21</t>
-  </si>
-  <si>
-    <t>scaling_factor</t>
-  </si>
-  <si>
-    <t>RealisePnLIncrease</t>
-  </si>
-  <si>
-    <t>RealisePnLDecrease</t>
-  </si>
-  <si>
-    <t>rpnlb_txn_001</t>
-  </si>
-  <si>
-    <t>rpnbl_txn_002</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -600,12 +600,12 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -617,111 +617,111 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
       </c>
       <c r="H2" s="3">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>99.5</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3">
-        <v>4975000</v>
+        <v>1000000</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>10000000</v>
+        <v>5000</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>99.5</v>
       </c>
       <c r="H5" s="3">
-        <v>50000</v>
+        <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -733,27 +733,27 @@
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
       </c>
       <c r="H6" s="3">
-        <v>4975000</v>
+        <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>22</v>
@@ -762,19 +762,19 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>325000</v>
+        <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -795,7 +795,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,13 +818,13 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -838,16 +838,16 @@
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -861,16 +861,16 @@
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
@@ -878,22 +878,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -907,16 +907,16 @@
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -930,16 +930,16 @@
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
@@ -947,22 +947,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
         <v>21</v>
@@ -976,16 +976,16 @@
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
@@ -993,45 +993,45 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
@@ -1045,16 +1045,16 @@
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -1068,16 +1068,16 @@
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>
@@ -1085,22 +1085,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -1114,16 +1114,16 @@
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1137,16 +1137,16 @@
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1154,22 +1154,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
@@ -1183,16 +1183,16 @@
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
         <v>23</v>
@@ -1200,45 +1200,45 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
SE-1843: Made several corrections and added additional explanations
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC7DDF2-1F91-4585-9EBE-7DAA401260E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9995F060-0B46-48C8-BEC5-F4FBC19DA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="0" yWindow="1068" windowWidth="23040" windowHeight="12360" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>tc</t>
-  </si>
-  <si>
     <t>2021-01-01T12:00:00Z</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>currency_id</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -172,13 +166,19 @@
     <t>rpnbl_txn_002</t>
   </si>
   <si>
-    <t>FutBob001</t>
-  </si>
-  <si>
-    <t>FutBob002</t>
-  </si>
-  <si>
     <t>futb_txn_001</t>
+  </si>
+  <si>
+    <t>FutBund001</t>
+  </si>
+  <si>
+    <t>FutBund002</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>total_commitment</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,36 +591,36 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
@@ -629,27 +629,27 @@
         <v>1000000</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1">
         <v>100</v>
@@ -658,27 +658,27 @@
         <v>1000000</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -687,27 +687,27 @@
         <v>5000</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G5" s="1">
         <v>99.5</v>
@@ -716,27 +716,27 @@
         <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
@@ -745,27 +745,27 @@
         <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -774,7 +774,7 @@
         <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -795,7 +795,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,430 +818,430 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1">
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F4" s="1">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F5" s="1">
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1">
         <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1">
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1">
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F9" s="1">
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F10" s="1">
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1">
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1">
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1">
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1">
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1">
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F17" s="1">
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F18" s="1">
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1">
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE-1843: Aligned sample transaction/quote dates based on Future maturity dates
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9995F060-0B46-48C8-BEC5-F4FBC19DA023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688D4763-6BDD-4415-939D-63009C65D42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1068" windowWidth="23040" windowHeight="12360" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -64,21 +64,9 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>2021-01-01T12:00:00Z</t>
-  </si>
-  <si>
     <t>OpenContract</t>
   </si>
   <si>
-    <t>2021-01-01T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T14:15:00Z</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -100,24 +88,12 @@
     <t>Day 2 closing price</t>
   </si>
   <si>
-    <t>2021-01-03T08:00:00Z</t>
-  </si>
-  <si>
     <t>Day 3 opening price</t>
   </si>
   <si>
     <t>Day 3 closing price</t>
   </si>
   <si>
-    <t>2021-01-01T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-03T17:00:00Z</t>
-  </si>
-  <si>
     <t>portfolio</t>
   </si>
   <si>
@@ -136,9 +112,6 @@
     <t>futb_txn_002</t>
   </si>
   <si>
-    <t>2021-01-03T14:15:00Z</t>
-  </si>
-  <si>
     <t>Day 3 intraday trade price</t>
   </si>
   <si>
@@ -179,6 +152,33 @@
   </si>
   <si>
     <t>total_commitment</t>
+  </si>
+  <si>
+    <t>2021-09-01T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T12:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T17:00:00Z</t>
   </si>
 </sst>
 </file>
@@ -560,9 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -591,36 +589,36 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
@@ -629,27 +627,27 @@
         <v>1000000</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
         <v>100</v>
@@ -658,27 +656,27 @@
         <v>1000000</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -687,27 +685,27 @@
         <v>5000</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1">
         <v>99.5</v>
@@ -716,27 +714,27 @@
         <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
@@ -745,27 +743,27 @@
         <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -774,7 +772,7 @@
         <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -795,7 +793,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,430 +816,430 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1">
-        <v>100</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1">
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1">
         <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1">
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1">
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1">
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1">
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
         <v>11</v>
-      </c>
-      <c r="B11">
-        <v>100</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1">
-        <v>100</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1">
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1">
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1">
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1">
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1">
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F19" s="1">
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE-1843: Futures PnL Cash Methodology Notebook with Bund Futures.
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B0DE4-1126-49D6-AB27-C17C0D1436C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688D4763-6BDD-4415-939D-63009C65D42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
@@ -64,24 +64,9 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>tc</t>
-  </si>
-  <si>
-    <t>2021-01-01T12:00:00Z</t>
-  </si>
-  <si>
     <t>OpenContract</t>
   </si>
   <si>
-    <t>2021-01-01T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T14:15:00Z</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -103,36 +88,18 @@
     <t>Day 2 closing price</t>
   </si>
   <si>
-    <t>2021-01-03T08:00:00Z</t>
-  </si>
-  <si>
     <t>Day 3 opening price</t>
   </si>
   <si>
     <t>Day 3 closing price</t>
   </si>
   <si>
-    <t>FUT_ICEKCZDEC21</t>
-  </si>
-  <si>
-    <t>2021-01-01T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-03T17:00:00Z</t>
-  </si>
-  <si>
     <t>portfolio</t>
   </si>
   <si>
     <t>currency_id</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -142,43 +109,76 @@
     <t>futa_txn_002</t>
   </si>
   <si>
+    <t>futb_txn_002</t>
+  </si>
+  <si>
+    <t>Day 3 intraday trade price</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>ClientInternal</t>
+  </si>
+  <si>
+    <t>FuturesPortfolioForPnLCalc</t>
+  </si>
+  <si>
+    <t>scaling_factor</t>
+  </si>
+  <si>
+    <t>RealisePnLIncrease</t>
+  </si>
+  <si>
+    <t>RealisePnLDecrease</t>
+  </si>
+  <si>
+    <t>rpnlb_txn_001</t>
+  </si>
+  <si>
+    <t>rpnbl_txn_002</t>
+  </si>
+  <si>
     <t>futb_txn_001</t>
   </si>
   <si>
-    <t>futb_txn_002</t>
-  </si>
-  <si>
-    <t>2021-01-03T14:15:00Z</t>
-  </si>
-  <si>
-    <t>Day 3 intraday trade price</t>
-  </si>
-  <si>
-    <t>id_type</t>
-  </si>
-  <si>
-    <t>ClientInternal</t>
-  </si>
-  <si>
-    <t>FuturesPortfolioForPnLCalc</t>
-  </si>
-  <si>
-    <t>FUT_ICEOJZDEC21</t>
-  </si>
-  <si>
-    <t>scaling_factor</t>
-  </si>
-  <si>
-    <t>RealisePnLIncrease</t>
-  </si>
-  <si>
-    <t>RealisePnLDecrease</t>
-  </si>
-  <si>
-    <t>rpnlb_txn_001</t>
-  </si>
-  <si>
-    <t>rpnbl_txn_002</t>
+    <t>FutBund001</t>
+  </si>
+  <si>
+    <t>FutBund002</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>total_commitment</t>
+  </si>
+  <si>
+    <t>2021-09-01T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T12:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T17:00:00Z</t>
   </si>
 </sst>
 </file>
@@ -560,9 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -591,45 +589,45 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
       </c>
       <c r="H2" s="3">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -637,144 +635,144 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1">
-        <v>99.5</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3">
-        <v>4975000</v>
+        <v>1000000</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
-        <v>10000000</v>
+        <v>5000</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>99.5</v>
       </c>
       <c r="H5" s="3">
-        <v>50000</v>
+        <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
       </c>
       <c r="H6" s="3">
-        <v>4975000</v>
+        <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>325000</v>
+        <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -795,7 +793,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,430 +816,430 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="1">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F19" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE-1843: Fixed several typos / wording errors
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688D4763-6BDD-4415-939D-63009C65D42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3F352-5989-4E7D-9E1B-CC5C48F6B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="0" yWindow="2304" windowWidth="23712" windowHeight="10044" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>total_commitment</t>
-  </si>
-  <si>
     <t>2021-09-01T08:00:00Z</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>2021-09-03T17:00:00Z</t>
+  </si>
+  <si>
+    <t>total_consideration</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -595,7 +597,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>19</v>
@@ -609,7 +611,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -638,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -667,7 +669,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -696,7 +698,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
@@ -725,7 +727,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
@@ -754,7 +756,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -830,7 +832,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -853,7 +855,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>100.5</v>
@@ -876,7 +878,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>100.5</v>
@@ -899,7 +901,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>100.5</v>
@@ -922,7 +924,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>99.5</v>
@@ -945,7 +947,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>98</v>
@@ -968,7 +970,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>98</v>
@@ -991,7 +993,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>104</v>
@@ -1014,7 +1016,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10">
         <v>104</v>
@@ -1037,7 +1039,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -1060,7 +1062,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>100.5</v>
@@ -1083,7 +1085,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>100.5</v>
@@ -1106,7 +1108,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>100.5</v>
@@ -1129,7 +1131,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>99.5</v>
@@ -1152,7 +1154,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>98</v>
@@ -1175,7 +1177,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>98</v>
@@ -1198,7 +1200,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>104</v>
@@ -1221,7 +1223,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>104</v>

</xml_diff>

<commit_message>
SE-1843: Renamed portfolio to better reflect example
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3F352-5989-4E7D-9E1B-CC5C48F6B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7CA25B-7C43-4579-B9B7-29326DE61AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2304" windowWidth="23712" windowHeight="10044" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>ClientInternal</t>
   </si>
   <si>
-    <t>FuturesPortfolioForPnLCalc</t>
-  </si>
-  <si>
     <t>scaling_factor</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>total_consideration</t>
+  </si>
+  <si>
+    <t>FuturesPortWithDiffCostBasis</t>
   </si>
 </sst>
 </file>
@@ -560,21 +560,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="4" width="23.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="23.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="23.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -597,13 +597,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -611,16 +611,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1">
         <v>100</v>
@@ -629,27 +629,27 @@
         <v>1000000</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1">
         <v>100</v>
@@ -658,27 +658,27 @@
         <v>1000000</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -687,10 +687,10 @@
         <v>5000</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -698,16 +698,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
         <v>99.5</v>
@@ -716,10 +716,10 @@
         <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -727,16 +727,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
@@ -745,27 +745,27 @@
         <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -774,13 +774,13 @@
         <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" s="4"/>
     </row>
   </sheetData>
@@ -798,16 +798,16 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -824,27 +824,27 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1">
         <v>100</v>
@@ -853,21 +853,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
         <v>100</v>
@@ -876,21 +876,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1">
         <v>100</v>
@@ -899,21 +899,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1">
         <v>100</v>
@@ -922,21 +922,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1">
         <v>100</v>
@@ -945,21 +945,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1">
         <v>100</v>
@@ -968,21 +968,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1">
         <v>100</v>
@@ -991,21 +991,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1">
         <v>100</v>
@@ -1014,21 +1014,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1">
         <v>100</v>
@@ -1037,21 +1037,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1">
         <v>100</v>
@@ -1060,21 +1060,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1">
         <v>100</v>
@@ -1083,21 +1083,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1">
         <v>100</v>
@@ -1106,21 +1106,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1">
         <v>100</v>
@@ -1129,21 +1129,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1">
         <v>100</v>
@@ -1152,21 +1152,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1">
         <v>100</v>
@@ -1175,21 +1175,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1">
         <v>100</v>
@@ -1198,21 +1198,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1">
         <v>100</v>
@@ -1221,21 +1221,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
SE-1843: Futures PnL Cash Methodology Notebook with Bund Futures. (#371)
* SE-1843: Futures PnL Cash Methodology Notebook with Bund Futures.

* SE-1843: Corrected cost basis for Dec contract and updated some descriptions

* SE-1843: Fixed several typos / wording errors

* SE-1843: Renamed portfolio to better reflect example
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/futures_data.xlsx
+++ b/examples/use-cases/valuation/data/futures_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\work\code\sample-notebooks\examples\use-cases\valuation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\thomaspartridge\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735B0DE4-1126-49D6-AB27-C17C0D1436C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7CA25B-7C43-4579-B9B7-29326DE61AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="1" r:id="rId1"/>
@@ -64,24 +64,9 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>tc</t>
-  </si>
-  <si>
-    <t>2021-01-01T12:00:00Z</t>
-  </si>
-  <si>
     <t>OpenContract</t>
   </si>
   <si>
-    <t>2021-01-01T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T08:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T14:15:00Z</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -103,36 +88,18 @@
     <t>Day 2 closing price</t>
   </si>
   <si>
-    <t>2021-01-03T08:00:00Z</t>
-  </si>
-  <si>
     <t>Day 3 opening price</t>
   </si>
   <si>
     <t>Day 3 closing price</t>
   </si>
   <si>
-    <t>FUT_ICEKCZDEC21</t>
-  </si>
-  <si>
-    <t>2021-01-01T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-02T17:00:00Z</t>
-  </si>
-  <si>
-    <t>2021-01-03T17:00:00Z</t>
-  </si>
-  <si>
     <t>portfolio</t>
   </si>
   <si>
     <t>currency_id</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>currency</t>
   </si>
   <si>
@@ -142,43 +109,76 @@
     <t>futa_txn_002</t>
   </si>
   <si>
+    <t>futb_txn_002</t>
+  </si>
+  <si>
+    <t>Day 3 intraday trade price</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>ClientInternal</t>
+  </si>
+  <si>
+    <t>scaling_factor</t>
+  </si>
+  <si>
+    <t>RealisePnLIncrease</t>
+  </si>
+  <si>
+    <t>RealisePnLDecrease</t>
+  </si>
+  <si>
+    <t>rpnlb_txn_001</t>
+  </si>
+  <si>
+    <t>rpnbl_txn_002</t>
+  </si>
+  <si>
     <t>futb_txn_001</t>
   </si>
   <si>
-    <t>futb_txn_002</t>
-  </si>
-  <si>
-    <t>2021-01-03T14:15:00Z</t>
-  </si>
-  <si>
-    <t>Day 3 intraday trade price</t>
-  </si>
-  <si>
-    <t>id_type</t>
-  </si>
-  <si>
-    <t>ClientInternal</t>
-  </si>
-  <si>
-    <t>FuturesPortfolioForPnLCalc</t>
-  </si>
-  <si>
-    <t>FUT_ICEOJZDEC21</t>
-  </si>
-  <si>
-    <t>scaling_factor</t>
-  </si>
-  <si>
-    <t>RealisePnLIncrease</t>
-  </si>
-  <si>
-    <t>RealisePnLDecrease</t>
-  </si>
-  <si>
-    <t>rpnlb_txn_001</t>
-  </si>
-  <si>
-    <t>rpnbl_txn_002</t>
+    <t>FutBund001</t>
+  </si>
+  <si>
+    <t>FutBund002</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>2021-09-01T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T08:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T12:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-01T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-02T17:00:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T14:15:00Z</t>
+  </si>
+  <si>
+    <t>2021-09-03T17:00:00Z</t>
+  </si>
+  <si>
+    <t>total_consideration</t>
+  </si>
+  <si>
+    <t>FuturesPortWithDiffCostBasis</t>
   </si>
 </sst>
 </file>
@@ -560,21 +560,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBDCCE7-B374-4F42-BF63-671E431676FC}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="4" width="23.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="23.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="23.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -591,196 +591,196 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1">
+        <v>100</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1">
-        <v>100</v>
-      </c>
-      <c r="H2" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1">
         <v>99.5</v>
       </c>
-      <c r="H3" s="3">
-        <v>4975000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1">
-        <v>100</v>
-      </c>
-      <c r="H4" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="I4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
       <c r="H5" s="3">
-        <v>50000</v>
+        <v>497500</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>99.5</v>
       </c>
       <c r="H6" s="3">
-        <v>4975000</v>
+        <v>497500</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
       <c r="H7" s="4">
-        <v>325000</v>
+        <v>32500</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" s="4"/>
     </row>
   </sheetData>
@@ -795,19 +795,19 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="33.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -818,430 +818,430 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>100.5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>100.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>100.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>99.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>98</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
       </c>
       <c r="B8">
         <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="1">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>100.5</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1">
+        <v>100</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>42</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>26</v>
       </c>
       <c r="B13">
         <v>100.5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>100.5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>99.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F15" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="1">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>40</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>22</v>
       </c>
       <c r="B17">
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F17" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1">
-        <v>1E-4</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>